<commit_message>
Code updated with cookie handling
</commit_message>
<xml_diff>
--- a/instamart_product_up.xlsx
+++ b/instamart_product_up.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -811,10 +811,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="D11" t="n">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -823,7 +823,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[[{'Variant Size': '84 g x 2', 'Price': '97', 'MRP': '140', 'Discount': '30% OFF', 'Status': 'In stock'}, {'Variant Size': '84 g', 'Price': '49', 'MRP': '70', 'Discount': '30% OFF', 'Status': 'In stock'}, {'Variant Size': '84 g x 3', 'Price': '141', 'MRP': '210', 'Discount': '32% OFF', 'Status': 'Sold Out'}]]</t>
+          <t>[['No variants']]</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -882,34 +882,390 @@
           <t>Go Zero</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="n">
+        <v>120</v>
+      </c>
+      <c r="D13" t="n">
+        <v>98</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Seller Name: Genuino Marketing Pvt Ltd - Pursaiwakam FSSAI Number: 20230922105165556 Address: FF Mekala Theatre building , door no 128 bricklin road Purasaiwalkam 600007</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>[[{'Variant Size': '100 ml x 4', 'Price': '379', 'MRP': '480', 'Discount': '21% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml x 2', 'Price': '192', 'MRP': '240', 'Discount': '20% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml', 'Price': '98', 'MRP': '120', 'Discount': '18% OFF', 'Status': 'In stock'}, {'Variant Size': '500 ml', 'Price': '327', 'MRP': '425', 'Discount': '23% OFF', 'Status': 'In stock'}]]</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://www.swiggy.com/instamart/item/YRL5V0ED04?storeId=1402050</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>600008</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>['Details not available for this location']</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>110006</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Go Zero Madagascar Chocobar Low Calorie Guilt Free Ice Cream Bar</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Go Zero</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Seller Name: PYD Retail Pvt Ltd - New Karol Bagh FSSAI Number: 20250325107131904 Address: UG Flr ,Plot 10130, Katra chajju pandit, main Rani Jhasi Road, New Delhi-110005</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>[[{'Variant Size': '60 ml x 4', 'Price': '400', 'MRP': '500', 'Discount': '20% OFF', 'Status': 'In stock'}, {'Variant Size': '60 ml x 2', 'Price': '202', 'MRP': '250', 'Discount': '19% OFF', 'Status': 'In stock'}, {'Variant Size': '60 ml', 'Price': '102', 'MRP': '125', 'Discount': '18% OFF', 'Status': 'In stock'}]]</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://www.swiggy.com/instamart/item/LNSIN80D9X?storeId=1402050</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>110006</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Go Zero Belgian Dark Chocolate Low Calorie Guilt Free Ice Cream Cup</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Go Zero</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>120</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>98</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Seller Name: Genuino Marketing Pvt Ltd - Pursaiwakam FSSAI Number: 20230922105165556 Address: FF Mekala Theatre building , door no 128 bricklin road Purasaiwalkam 600007</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>[[{'Variant Size': '100 ml x 4', 'Price': '379', 'MRP': '480', 'Discount': '21% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml x 2', 'Price': '192', 'MRP': '240', 'Discount': '20% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml', 'Price': '98', 'MRP': '120', 'Discount': '18% OFF', 'Status': 'In stock'}, {'Variant Size': '500 ml', 'Price': '327', 'MRP': '425', 'Discount': '23% OFF', 'Status': 'In stock'}]]</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Seller Name: PYD Retail Pvt Ltd - New Karol Bagh FSSAI Number: 20250325107131904 Address: UG Flr ,Plot 10130, Katra chajju pandit, main Rani Jhasi Road, New Delhi-110005</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>[[{'Variant Size': '500 ml', 'Price': '327', 'MRP': '425', 'Discount': '23% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml x 4', 'Price': '379', 'MRP': '480', 'Discount': '21% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml', 'Price': '98', 'MRP': '120', 'Discount': '18% OFF', 'Status': 'In stock'}]]</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>https://www.swiggy.com/instamart/item/YRL5V0ED04?storeId=1402050</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>600008</t>
+      <c r="H16" t="n">
+        <v>110006</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>['Details not available for this location']</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Details not available for this location</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>110008</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Go Zero Madagascar Chocobar Low Calorie Guilt Free Ice Cream Bar</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Go Zero</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Seller Name: PYD Retail Pvt. Ltd. Patel Nagar FSSAI Number: 13322006000126 Address: Plot No BP-08,West Patel Nagar,New Delhi-110008</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>[[{'Variant Size': '60 ml x 4', 'Price': '400', 'MRP': '500', 'Discount': '20% OFF', 'Status': 'In stock'}, {'Variant Size': '60 ml x 2', 'Price': '202', 'MRP': '250', 'Discount': '19% OFF', 'Status': 'In stock'}, {'Variant Size': '60 ml', 'Price': '102', 'MRP': '125', 'Discount': '18% OFF', 'Status': 'In stock'}]]</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>https://www.swiggy.com/instamart/item/LNSIN80D9X?storeId=1402050</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>110008</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Go Zero Belgian Dark Chocolate Low Calorie Guilt Free Ice Cream Cup</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Go Zero</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Seller Name: PYD Retail Pvt. Ltd. Patel Nagar FSSAI Number: 13322006000126 Address: Plot No BP-08,West Patel Nagar,New Delhi-110008</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>[[{'Variant Size': '500 ml', 'Price': '327', 'MRP': '425', 'Discount': '23% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml x 4', 'Price': '379', 'MRP': '480', 'Discount': '21% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml', 'Price': '98', 'MRP': '120', 'Discount': '18% OFF', 'Status': 'In stock'}]]</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>https://www.swiggy.com/instamart/item/YRL5V0ED04?storeId=1402050</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>110008</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Too Yumm! Chips Indian Masala</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Too Yumm!</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Seller Name: PYD Retail Pvt Ltd - Jharsa Village FSSAI Number: 20250116106886225 Address: GF, B-12, sector-45, near greenwood city, Gurgaon-122003</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>[['No variants']]</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>https://www.swiggy.com/instamart/item/N5SBE9SBEE?storeId=1402050</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>122003</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Go Zero Madagascar Chocobar Low Calorie Guilt Free Ice Cream Bar</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Go Zero</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>109</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Seller Name: PYD Retail Pvt Ltd - Sector 50 FSSAI Number: 20240903106414148 Address: U.no 105,106,108, 04, 110-112, gf to 7th floor Revenue Estate of Village Badshahpur, Sector 50, Gurgaon, Haryana, 122108</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>[[{'Variant Size': '60 ml x 2', 'Price': '202', 'MRP': '250', 'Discount': '19% OFF', 'Status': 'In stock'}, {'Variant Size': '60 ml', 'Price': '102', 'MRP': '125', 'Discount': '18% OFF', 'Status': 'In stock'}]]</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>https://www.swiggy.com/instamart/item/LNSIN80D9X?storeId=1402050</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>122003</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Go Zero Belgian Dark Chocolate Low Calorie Guilt Free Ice Cream Cup</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Go Zero</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>425</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>327</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Seller Name: PYD Retail Pvt Ltd - Sector 50 FSSAI Number: 20240903106414148 Address: U.no 105,106,108, 04, 110-112, gf to 7th floor Revenue Estate of Village Badshahpur, Sector 50, Gurgaon, Haryana, 122108</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>[[{'Variant Size': '500 ml', 'Price': '327', 'MRP': '425', 'Discount': '23% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml x 4', 'Price': '379', 'MRP': '480', 'Discount': '21% OFF', 'Status': 'In stock'}, {'Variant Size': '100 ml', 'Price': '98', 'MRP': '120', 'Discount': '18% OFF', 'Status': 'Sold Out'}]]</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>https://www.swiggy.com/instamart/item/YRL5V0ED04?storeId=1402050</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>122003</t>
         </is>
       </c>
     </row>

</xml_diff>